<commit_message>
Spreadsheets and Graphs fix
</commit_message>
<xml_diff>
--- a/Project 2/FractionsTimingSpreadsheet.xlsx
+++ b/Project 2/FractionsTimingSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan C\Documents\GitHub\IT310\Project 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB2C94E-4366-4DA9-95F7-F47F36B30A93}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE191D0E-6BA3-4761-A6E1-12DC36E49B1B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{688989AF-19A3-4C8D-B96D-41811F89DBF4}"/>
   </bookViews>
@@ -233,10 +233,10 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
+                  <c:v>Insertion Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Selection Sort</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Insertion Sort</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Bubble Sort</c:v>
@@ -319,10 +319,10 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
+                  <c:v>Insertion Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Selection Sort</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Insertion Sort</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Bubble Sort</c:v>
@@ -405,10 +405,10 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
+                  <c:v>Insertion Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Selection Sort</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Insertion Sort</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Bubble Sort</c:v>
@@ -491,10 +491,10 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
+                  <c:v>Insertion Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Selection Sort</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Insertion Sort</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Bubble Sort</c:v>
@@ -1377,15 +1377,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1712,9 +1712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48DE1230-03C1-491E-A018-8CBCCE180CE0}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1726,10 +1724,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>

</xml_diff>